<commit_message>
Initial commit for  APP model
</commit_message>
<xml_diff>
--- a/Daily_Bets/19.07.2025.xlsx
+++ b/Daily_Bets/19.07.2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/91e7899ff25e1dfc/Python/V3/Ripon/Daily_Bets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/91e7899ff25e1dfc/Python/App/Daily_Bets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="11_3FFB71EBC3CC1986E1EE60FE71F93EB925D4E046" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48D49992-D378-CA42-AA2A-94330E5A85C6}"/>
+  <xr:revisionPtr revIDLastSave="239" documentId="11_3FFB71EBC3CC1986E1EE60FE71F93EB925D4E046" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A66E71CE-D65E-4757-AF45-F60E0A71FBB2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1667,6 +1667,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2022,72 +2026,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BE193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J75" workbookViewId="0">
-      <selection activeCell="S111" sqref="S111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.296875" customWidth="1"/>
-    <col min="3" max="3" width="13.31640625" customWidth="1"/>
-    <col min="4" max="4" width="9.55078125" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.8359375" customWidth="1"/>
-    <col min="7" max="7" width="8.875" customWidth="1"/>
-    <col min="8" max="8" width="8.7421875" customWidth="1"/>
-    <col min="9" max="9" width="8.203125" customWidth="1"/>
-    <col min="10" max="10" width="14.66015625" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
     <col min="11" max="11" width="4.5703125" customWidth="1"/>
-    <col min="12" max="12" width="3.2265625" customWidth="1"/>
-    <col min="13" max="13" width="3.765625" customWidth="1"/>
-    <col min="14" max="14" width="4.16796875" customWidth="1"/>
-    <col min="15" max="15" width="7.12890625" customWidth="1"/>
-    <col min="16" max="16" width="15.19921875" customWidth="1"/>
-    <col min="17" max="17" width="5.37890625" customWidth="1"/>
-    <col min="18" max="18" width="4.4375" customWidth="1"/>
-    <col min="19" max="19" width="8.7421875" customWidth="1"/>
-    <col min="20" max="20" width="12.9140625" customWidth="1"/>
-    <col min="21" max="21" width="9.953125" customWidth="1"/>
-    <col min="22" max="22" width="10.22265625" customWidth="1"/>
-    <col min="23" max="23" width="11.296875" customWidth="1"/>
-    <col min="24" max="24" width="11.56640625" customWidth="1"/>
-    <col min="25" max="25" width="18.83203125" customWidth="1"/>
-    <col min="26" max="26" width="9.01171875" customWidth="1"/>
-    <col min="27" max="27" width="19.37109375" customWidth="1"/>
-    <col min="28" max="28" width="11.56640625" customWidth="1"/>
-    <col min="29" max="29" width="16.8125" customWidth="1"/>
-    <col min="30" max="30" width="14.52734375" customWidth="1"/>
-    <col min="31" max="31" width="20.58203125" customWidth="1"/>
-    <col min="32" max="32" width="16.54296875" customWidth="1"/>
-    <col min="33" max="33" width="15.46875" customWidth="1"/>
-    <col min="34" max="34" width="18.4296875" customWidth="1"/>
-    <col min="35" max="35" width="17.21875" customWidth="1"/>
-    <col min="36" max="36" width="19.90625" customWidth="1"/>
-    <col min="37" max="37" width="21.65625" customWidth="1"/>
-    <col min="38" max="38" width="19.1015625" customWidth="1"/>
-    <col min="39" max="39" width="27.3046875" customWidth="1"/>
+    <col min="12" max="12" width="3.28515625" customWidth="1"/>
+    <col min="13" max="13" width="3.7109375" customWidth="1"/>
+    <col min="14" max="14" width="4.140625" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" customWidth="1"/>
+    <col min="17" max="17" width="5.42578125" customWidth="1"/>
+    <col min="18" max="18" width="4.42578125" customWidth="1"/>
+    <col min="19" max="19" width="8.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12.85546875" customWidth="1"/>
+    <col min="21" max="21" width="10" customWidth="1"/>
+    <col min="22" max="22" width="10.28515625" customWidth="1"/>
+    <col min="23" max="23" width="11.28515625" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" customWidth="1"/>
+    <col min="25" max="25" width="18.85546875" customWidth="1"/>
+    <col min="26" max="26" width="9" customWidth="1"/>
+    <col min="27" max="27" width="19.42578125" customWidth="1"/>
+    <col min="28" max="28" width="11.5703125" customWidth="1"/>
+    <col min="29" max="29" width="16.85546875" customWidth="1"/>
+    <col min="30" max="30" width="14.5703125" customWidth="1"/>
+    <col min="31" max="31" width="20.5703125" customWidth="1"/>
+    <col min="32" max="32" width="16.5703125" customWidth="1"/>
+    <col min="33" max="33" width="15.42578125" customWidth="1"/>
+    <col min="34" max="34" width="18.42578125" customWidth="1"/>
+    <col min="35" max="35" width="17.28515625" customWidth="1"/>
+    <col min="36" max="36" width="19.85546875" customWidth="1"/>
+    <col min="37" max="37" width="21.7109375" customWidth="1"/>
+    <col min="38" max="38" width="19.140625" customWidth="1"/>
+    <col min="39" max="39" width="27.28515625" customWidth="1"/>
     <col min="40" max="40" width="27.7109375" customWidth="1"/>
-    <col min="41" max="41" width="13.98828125" customWidth="1"/>
-    <col min="42" max="42" width="12.64453125" customWidth="1"/>
-    <col min="43" max="43" width="18.5625" customWidth="1"/>
-    <col min="44" max="44" width="25.15234375" customWidth="1"/>
-    <col min="45" max="45" width="15.19921875" customWidth="1"/>
-    <col min="46" max="46" width="16.54296875" customWidth="1"/>
-    <col min="47" max="47" width="13.5859375" customWidth="1"/>
-    <col min="48" max="48" width="14.2578125" customWidth="1"/>
+    <col min="41" max="41" width="14" customWidth="1"/>
+    <col min="42" max="42" width="12.7109375" customWidth="1"/>
+    <col min="43" max="43" width="18.5703125" customWidth="1"/>
+    <col min="44" max="44" width="25.140625" customWidth="1"/>
+    <col min="45" max="45" width="15.140625" customWidth="1"/>
+    <col min="46" max="46" width="16.5703125" customWidth="1"/>
+    <col min="47" max="47" width="13.5703125" customWidth="1"/>
+    <col min="48" max="48" width="14.28515625" customWidth="1"/>
     <col min="49" max="49" width="23" customWidth="1"/>
-    <col min="50" max="50" width="17.21875" customWidth="1"/>
-    <col min="51" max="51" width="18.6953125" customWidth="1"/>
-    <col min="52" max="52" width="12.9140625" customWidth="1"/>
-    <col min="53" max="53" width="17.75390625" customWidth="1"/>
-    <col min="54" max="54" width="25.15234375" customWidth="1"/>
-    <col min="55" max="55" width="15.33203125" customWidth="1"/>
-    <col min="56" max="56" width="18.6953125" customWidth="1"/>
-    <col min="57" max="57" width="14.9296875" customWidth="1"/>
+    <col min="50" max="50" width="17.28515625" customWidth="1"/>
+    <col min="51" max="51" width="18.7109375" customWidth="1"/>
+    <col min="52" max="52" width="12.85546875" customWidth="1"/>
+    <col min="53" max="53" width="17.7109375" customWidth="1"/>
+    <col min="54" max="54" width="25.140625" customWidth="1"/>
+    <col min="55" max="55" width="15.28515625" customWidth="1"/>
+    <col min="56" max="56" width="18.7109375" customWidth="1"/>
+    <col min="57" max="57" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2260,7 +2264,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45857</v>
       </c>
@@ -2415,7 +2419,7 @@
       </c>
       <c r="BE2" s="2"/>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45857</v>
       </c>
@@ -2570,7 +2574,7 @@
       </c>
       <c r="BE3" s="2"/>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45857</v>
       </c>
@@ -2725,7 +2729,7 @@
       </c>
       <c r="BE4" s="2"/>
     </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45857</v>
       </c>
@@ -2880,7 +2884,7 @@
       </c>
       <c r="BE5" s="2"/>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45857</v>
       </c>
@@ -3035,7 +3039,7 @@
       </c>
       <c r="BE6" s="2"/>
     </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45857</v>
       </c>
@@ -3190,7 +3194,7 @@
       </c>
       <c r="BE7" s="2"/>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45857</v>
       </c>
@@ -3345,7 +3349,7 @@
       </c>
       <c r="BE8" s="2"/>
     </row>
-    <row r="9" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>45857</v>
       </c>
@@ -3500,7 +3504,7 @@
       </c>
       <c r="BE9" s="8"/>
     </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45857</v>
       </c>
@@ -3655,7 +3659,7 @@
       </c>
       <c r="BE10" s="2"/>
     </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45857</v>
       </c>
@@ -3810,7 +3814,7 @@
       </c>
       <c r="BE11" s="2"/>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45857</v>
       </c>
@@ -3965,7 +3969,7 @@
       </c>
       <c r="BE12" s="2"/>
     </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45857</v>
       </c>
@@ -4120,7 +4124,7 @@
       </c>
       <c r="BE13" s="2"/>
     </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45857</v>
       </c>
@@ -4275,7 +4279,7 @@
       </c>
       <c r="BE14" s="2"/>
     </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45857</v>
       </c>
@@ -4430,7 +4434,7 @@
       </c>
       <c r="BE15" s="2"/>
     </row>
-    <row r="16" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>45857</v>
       </c>
@@ -4585,7 +4589,7 @@
       </c>
       <c r="BE16" s="8"/>
     </row>
-    <row r="17" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45857</v>
       </c>
@@ -4740,7 +4744,7 @@
       </c>
       <c r="BE17" s="2"/>
     </row>
-    <row r="18" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45857</v>
       </c>
@@ -4895,7 +4899,7 @@
       </c>
       <c r="BE18" s="2"/>
     </row>
-    <row r="19" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45857</v>
       </c>
@@ -5050,7 +5054,7 @@
       </c>
       <c r="BE19" s="2"/>
     </row>
-    <row r="20" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45857</v>
       </c>
@@ -5205,7 +5209,7 @@
       </c>
       <c r="BE20" s="2"/>
     </row>
-    <row r="21" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45857</v>
       </c>
@@ -5360,7 +5364,7 @@
       </c>
       <c r="BE21" s="2"/>
     </row>
-    <row r="22" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45857</v>
       </c>
@@ -5515,7 +5519,7 @@
       </c>
       <c r="BE22" s="2"/>
     </row>
-    <row r="23" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45857</v>
       </c>
@@ -5670,7 +5674,7 @@
       </c>
       <c r="BE23" s="2"/>
     </row>
-    <row r="24" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45857</v>
       </c>
@@ -5825,7 +5829,7 @@
       </c>
       <c r="BE24" s="2"/>
     </row>
-    <row r="25" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45857</v>
       </c>
@@ -5980,7 +5984,7 @@
       </c>
       <c r="BE25" s="2"/>
     </row>
-    <row r="26" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45857</v>
       </c>
@@ -6135,7 +6139,7 @@
       </c>
       <c r="BE26" s="2"/>
     </row>
-    <row r="27" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45857</v>
       </c>
@@ -6290,7 +6294,7 @@
       </c>
       <c r="BE27" s="2"/>
     </row>
-    <row r="28" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45857</v>
       </c>
@@ -6445,7 +6449,7 @@
       </c>
       <c r="BE28" s="2"/>
     </row>
-    <row r="29" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45857</v>
       </c>
@@ -6600,7 +6604,7 @@
       </c>
       <c r="BE29" s="2"/>
     </row>
-    <row r="30" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45857</v>
       </c>
@@ -6755,7 +6759,7 @@
       </c>
       <c r="BE30" s="2"/>
     </row>
-    <row r="31" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45857</v>
       </c>
@@ -6910,7 +6914,7 @@
       </c>
       <c r="BE31" s="2"/>
     </row>
-    <row r="32" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45857</v>
       </c>
@@ -7065,7 +7069,7 @@
       </c>
       <c r="BE32" s="2"/>
     </row>
-    <row r="33" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45857</v>
       </c>
@@ -7220,7 +7224,7 @@
       </c>
       <c r="BE33" s="2"/>
     </row>
-    <row r="34" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>45857</v>
       </c>
@@ -7375,7 +7379,7 @@
       </c>
       <c r="BE34" s="2"/>
     </row>
-    <row r="35" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>45857</v>
       </c>
@@ -7530,7 +7534,7 @@
       </c>
       <c r="BE35" s="2"/>
     </row>
-    <row r="36" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>45857</v>
       </c>
@@ -7685,7 +7689,7 @@
       </c>
       <c r="BE36" s="2"/>
     </row>
-    <row r="37" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>45857</v>
       </c>
@@ -7840,7 +7844,7 @@
       </c>
       <c r="BE37" s="2"/>
     </row>
-    <row r="38" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>45857</v>
       </c>
@@ -7995,7 +7999,7 @@
       </c>
       <c r="BE38" s="2"/>
     </row>
-    <row r="39" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>45857</v>
       </c>
@@ -8150,7 +8154,7 @@
       </c>
       <c r="BE39" s="2"/>
     </row>
-    <row r="40" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>45857</v>
       </c>
@@ -8305,7 +8309,7 @@
       </c>
       <c r="BE40" s="2"/>
     </row>
-    <row r="41" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>45857</v>
       </c>
@@ -8460,7 +8464,7 @@
       </c>
       <c r="BE41" s="2"/>
     </row>
-    <row r="42" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>45857</v>
       </c>
@@ -8615,7 +8619,7 @@
       </c>
       <c r="BE42" s="2"/>
     </row>
-    <row r="43" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>45857</v>
       </c>
@@ -8770,7 +8774,7 @@
       </c>
       <c r="BE43" s="2"/>
     </row>
-    <row r="44" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>45857</v>
       </c>
@@ -8925,7 +8929,7 @@
       </c>
       <c r="BE44" s="2"/>
     </row>
-    <row r="45" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>45857</v>
       </c>
@@ -9080,7 +9084,7 @@
       </c>
       <c r="BE45" s="2"/>
     </row>
-    <row r="46" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45857</v>
       </c>
@@ -9235,7 +9239,7 @@
       </c>
       <c r="BE46" s="2"/>
     </row>
-    <row r="47" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45857</v>
       </c>
@@ -9390,7 +9394,7 @@
       </c>
       <c r="BE47" s="2"/>
     </row>
-    <row r="48" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>45857</v>
       </c>
@@ -9545,7 +9549,7 @@
       </c>
       <c r="BE48" s="8"/>
     </row>
-    <row r="49" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45857</v>
       </c>
@@ -9697,7 +9701,7 @@
       </c>
       <c r="BE49" s="2"/>
     </row>
-    <row r="50" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>45857</v>
       </c>
@@ -9852,7 +9856,7 @@
       </c>
       <c r="BE50" s="2"/>
     </row>
-    <row r="51" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>45857</v>
       </c>
@@ -10007,7 +10011,7 @@
       </c>
       <c r="BE51" s="2"/>
     </row>
-    <row r="52" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>45857</v>
       </c>
@@ -10162,7 +10166,7 @@
       </c>
       <c r="BE52" s="2"/>
     </row>
-    <row r="53" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>45857</v>
       </c>
@@ -10317,7 +10321,7 @@
       </c>
       <c r="BE53" s="2"/>
     </row>
-    <row r="54" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>45857</v>
       </c>
@@ -10472,7 +10476,7 @@
       </c>
       <c r="BE54" s="2"/>
     </row>
-    <row r="55" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>45857</v>
       </c>
@@ -10627,7 +10631,7 @@
       </c>
       <c r="BE55" s="2"/>
     </row>
-    <row r="56" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>45857</v>
       </c>
@@ -10782,7 +10786,7 @@
       </c>
       <c r="BE56" s="8"/>
     </row>
-    <row r="57" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>45857</v>
       </c>
@@ -10937,7 +10941,7 @@
       </c>
       <c r="BE57" s="2"/>
     </row>
-    <row r="58" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>45857</v>
       </c>
@@ -11089,7 +11093,7 @@
       </c>
       <c r="BE58" s="2"/>
     </row>
-    <row r="59" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>45857</v>
       </c>
@@ -11241,7 +11245,7 @@
       </c>
       <c r="BE59" s="2"/>
     </row>
-    <row r="60" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>45857</v>
       </c>
@@ -11393,7 +11397,7 @@
       </c>
       <c r="BE60" s="2"/>
     </row>
-    <row r="61" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>45857</v>
       </c>
@@ -11545,7 +11549,7 @@
       </c>
       <c r="BE61" s="2"/>
     </row>
-    <row r="62" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>45857</v>
       </c>
@@ -11700,7 +11704,7 @@
       </c>
       <c r="BE62" s="8"/>
     </row>
-    <row r="63" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>45857</v>
       </c>
@@ -11855,7 +11859,7 @@
       </c>
       <c r="BE63" s="2"/>
     </row>
-    <row r="64" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>45857</v>
       </c>
@@ -12010,7 +12014,7 @@
       </c>
       <c r="BE64" s="2"/>
     </row>
-    <row r="65" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>45857</v>
       </c>
@@ -12165,7 +12169,7 @@
       </c>
       <c r="BE65" s="2"/>
     </row>
-    <row r="66" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>45857</v>
       </c>
@@ -12320,7 +12324,7 @@
       </c>
       <c r="BE66" s="2"/>
     </row>
-    <row r="67" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>45857</v>
       </c>
@@ -12475,7 +12479,7 @@
       </c>
       <c r="BE67" s="2"/>
     </row>
-    <row r="68" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>45857</v>
       </c>
@@ -12630,7 +12634,7 @@
       </c>
       <c r="BE68" s="2"/>
     </row>
-    <row r="69" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>45857</v>
       </c>
@@ -12785,7 +12789,7 @@
       </c>
       <c r="BE69" s="2"/>
     </row>
-    <row r="70" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>45857</v>
       </c>
@@ -12940,7 +12944,7 @@
       </c>
       <c r="BE70" s="2"/>
     </row>
-    <row r="71" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>45857</v>
       </c>
@@ -13095,7 +13099,7 @@
       </c>
       <c r="BE71" s="2"/>
     </row>
-    <row r="72" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>45857</v>
       </c>
@@ -13247,7 +13251,7 @@
       </c>
       <c r="BE72" s="2"/>
     </row>
-    <row r="73" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>45857</v>
       </c>
@@ -13402,7 +13406,7 @@
       </c>
       <c r="BE73" s="2"/>
     </row>
-    <row r="74" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>45857</v>
       </c>
@@ -13557,7 +13561,7 @@
       </c>
       <c r="BE74" s="2"/>
     </row>
-    <row r="75" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>45857</v>
       </c>
@@ -13709,7 +13713,7 @@
       </c>
       <c r="BE75" s="2"/>
     </row>
-    <row r="76" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>45857</v>
       </c>
@@ -13861,7 +13865,7 @@
       </c>
       <c r="BE76" s="2"/>
     </row>
-    <row r="77" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>45857</v>
       </c>
@@ -14013,7 +14017,7 @@
       </c>
       <c r="BE77" s="2"/>
     </row>
-    <row r="78" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>45857</v>
       </c>
@@ -14168,7 +14172,7 @@
       </c>
       <c r="BE78" s="2"/>
     </row>
-    <row r="79" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>45857</v>
       </c>
@@ -14323,7 +14327,7 @@
       </c>
       <c r="BE79" s="2"/>
     </row>
-    <row r="80" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>45857</v>
       </c>
@@ -14475,7 +14479,7 @@
       </c>
       <c r="BE80" s="2"/>
     </row>
-    <row r="81" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>45857</v>
       </c>
@@ -14630,7 +14634,7 @@
       </c>
       <c r="BE81" s="2"/>
     </row>
-    <row r="82" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>45857</v>
       </c>
@@ -14782,7 +14786,7 @@
       </c>
       <c r="BE82" s="2"/>
     </row>
-    <row r="83" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>45857</v>
       </c>
@@ -14937,7 +14941,7 @@
       </c>
       <c r="BE83" s="2"/>
     </row>
-    <row r="84" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>45857</v>
       </c>
@@ -15092,7 +15096,7 @@
       </c>
       <c r="BE84" s="2"/>
     </row>
-    <row r="85" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>45857</v>
       </c>
@@ -15247,7 +15251,7 @@
       </c>
       <c r="BE85" s="2"/>
     </row>
-    <row r="86" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>45857</v>
       </c>
@@ -15402,7 +15406,7 @@
       </c>
       <c r="BE86" s="2"/>
     </row>
-    <row r="87" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>45857</v>
       </c>
@@ -15557,7 +15561,7 @@
       </c>
       <c r="BE87" s="2"/>
     </row>
-    <row r="88" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>45857</v>
       </c>
@@ -15712,7 +15716,7 @@
       </c>
       <c r="BE88" s="2"/>
     </row>
-    <row r="89" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>45857</v>
       </c>
@@ -15867,7 +15871,7 @@
       </c>
       <c r="BE89" s="2"/>
     </row>
-    <row r="90" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>45857</v>
       </c>
@@ -16022,7 +16026,7 @@
       </c>
       <c r="BE90" s="2"/>
     </row>
-    <row r="91" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>45857</v>
       </c>
@@ -16177,7 +16181,7 @@
       </c>
       <c r="BE91" s="2"/>
     </row>
-    <row r="92" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>45857</v>
       </c>
@@ -16332,7 +16336,7 @@
       </c>
       <c r="BE92" s="2"/>
     </row>
-    <row r="93" spans="1:57" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:57" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12">
         <v>45857</v>
       </c>
@@ -16487,7 +16491,7 @@
       </c>
       <c r="BE93" s="14"/>
     </row>
-    <row r="94" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>45857</v>
       </c>
@@ -16642,7 +16646,7 @@
       </c>
       <c r="BE94" s="2"/>
     </row>
-    <row r="95" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>45857</v>
       </c>
@@ -16797,7 +16801,7 @@
       </c>
       <c r="BE95" s="2"/>
     </row>
-    <row r="96" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>45857</v>
       </c>
@@ -16952,7 +16956,7 @@
       </c>
       <c r="BE96" s="2"/>
     </row>
-    <row r="97" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>45857</v>
       </c>
@@ -17107,7 +17111,7 @@
       </c>
       <c r="BE97" s="2"/>
     </row>
-    <row r="98" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>45857</v>
       </c>
@@ -17262,7 +17266,7 @@
       </c>
       <c r="BE98" s="2"/>
     </row>
-    <row r="99" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6">
         <v>45857</v>
       </c>
@@ -17417,7 +17421,7 @@
       </c>
       <c r="BE99" s="8"/>
     </row>
-    <row r="100" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>45857</v>
       </c>
@@ -17572,7 +17576,7 @@
       </c>
       <c r="BE100" s="2"/>
     </row>
-    <row r="101" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>45857</v>
       </c>
@@ -17727,7 +17731,7 @@
       </c>
       <c r="BE101" s="2"/>
     </row>
-    <row r="102" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>45857</v>
       </c>
@@ -17882,7 +17886,7 @@
       </c>
       <c r="BE102" s="2"/>
     </row>
-    <row r="103" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>45857</v>
       </c>
@@ -18037,7 +18041,7 @@
       </c>
       <c r="BE103" s="2"/>
     </row>
-    <row r="104" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>45857</v>
       </c>
@@ -18192,7 +18196,7 @@
       </c>
       <c r="BE104" s="2"/>
     </row>
-    <row r="105" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>45857</v>
       </c>
@@ -18347,7 +18351,7 @@
       </c>
       <c r="BE105" s="2"/>
     </row>
-    <row r="106" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>45857</v>
       </c>
@@ -18502,7 +18506,7 @@
       </c>
       <c r="BE106" s="2"/>
     </row>
-    <row r="107" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>45857</v>
       </c>
@@ -18657,7 +18661,7 @@
       </c>
       <c r="BE107" s="2"/>
     </row>
-    <row r="108" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>45857</v>
       </c>
@@ -18812,7 +18816,7 @@
       </c>
       <c r="BE108" s="2"/>
     </row>
-    <row r="109" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>45857</v>
       </c>
@@ -18967,7 +18971,7 @@
       </c>
       <c r="BE109" s="2"/>
     </row>
-    <row r="110" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>45857</v>
       </c>
@@ -19122,7 +19126,7 @@
       </c>
       <c r="BE110" s="2"/>
     </row>
-    <row r="111" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>45857</v>
       </c>
@@ -19277,7 +19281,7 @@
       </c>
       <c r="BE111" s="2"/>
     </row>
-    <row r="112" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>45857</v>
       </c>
@@ -19432,7 +19436,7 @@
       </c>
       <c r="BE112" s="2"/>
     </row>
-    <row r="113" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>45857</v>
       </c>
@@ -19587,7 +19591,7 @@
       </c>
       <c r="BE113" s="2"/>
     </row>
-    <row r="114" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>45857</v>
       </c>
@@ -19742,7 +19746,7 @@
       </c>
       <c r="BE114" s="2"/>
     </row>
-    <row r="115" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>45857</v>
       </c>
@@ -19897,7 +19901,7 @@
       </c>
       <c r="BE115" s="2"/>
     </row>
-    <row r="116" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>45857</v>
       </c>
@@ -20052,7 +20056,7 @@
       </c>
       <c r="BE116" s="2"/>
     </row>
-    <row r="117" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>45857</v>
       </c>
@@ -20207,7 +20211,7 @@
       </c>
       <c r="BE117" s="2"/>
     </row>
-    <row r="118" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>45857</v>
       </c>
@@ -20362,7 +20366,7 @@
       </c>
       <c r="BE118" s="2"/>
     </row>
-    <row r="119" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>45857</v>
       </c>
@@ -20517,7 +20521,7 @@
       </c>
       <c r="BE119" s="2"/>
     </row>
-    <row r="120" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>45857</v>
       </c>
@@ -20669,7 +20673,7 @@
       </c>
       <c r="BE120" s="2"/>
     </row>
-    <row r="121" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>45857</v>
       </c>
@@ -20824,7 +20828,7 @@
       </c>
       <c r="BE121" s="2"/>
     </row>
-    <row r="122" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>45857</v>
       </c>
@@ -20979,7 +20983,7 @@
       </c>
       <c r="BE122" s="2"/>
     </row>
-    <row r="123" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>45857</v>
       </c>
@@ -21134,7 +21138,7 @@
       </c>
       <c r="BE123" s="2"/>
     </row>
-    <row r="124" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>45857</v>
       </c>
@@ -21289,7 +21293,7 @@
       </c>
       <c r="BE124" s="2"/>
     </row>
-    <row r="125" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>45857</v>
       </c>
@@ -21444,7 +21448,7 @@
       </c>
       <c r="BE125" s="2"/>
     </row>
-    <row r="126" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>45857</v>
       </c>
@@ -21599,7 +21603,7 @@
       </c>
       <c r="BE126" s="2"/>
     </row>
-    <row r="127" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>45857</v>
       </c>
@@ -21754,7 +21758,7 @@
       </c>
       <c r="BE127" s="2"/>
     </row>
-    <row r="128" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>45857</v>
       </c>
@@ -21909,7 +21913,7 @@
       </c>
       <c r="BE128" s="2"/>
     </row>
-    <row r="129" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>45857</v>
       </c>
@@ -22064,7 +22068,7 @@
       </c>
       <c r="BE129" s="2"/>
     </row>
-    <row r="130" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>45857</v>
       </c>
@@ -22219,7 +22223,7 @@
       </c>
       <c r="BE130" s="2"/>
     </row>
-    <row r="131" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>45857</v>
       </c>
@@ -22374,7 +22378,7 @@
       </c>
       <c r="BE131" s="2"/>
     </row>
-    <row r="132" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>45857</v>
       </c>
@@ -22529,7 +22533,7 @@
       </c>
       <c r="BE132" s="2"/>
     </row>
-    <row r="133" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>45857</v>
       </c>
@@ -22684,7 +22688,7 @@
       </c>
       <c r="BE133" s="2"/>
     </row>
-    <row r="134" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>45857</v>
       </c>
@@ -22839,7 +22843,7 @@
       </c>
       <c r="BE134" s="2"/>
     </row>
-    <row r="135" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>45857</v>
       </c>
@@ -22994,7 +22998,7 @@
       </c>
       <c r="BE135" s="2"/>
     </row>
-    <row r="136" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>45857</v>
       </c>
@@ -23149,7 +23153,7 @@
       </c>
       <c r="BE136" s="2"/>
     </row>
-    <row r="137" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>45857</v>
       </c>
@@ -23304,7 +23308,7 @@
       </c>
       <c r="BE137" s="2"/>
     </row>
-    <row r="138" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>45857</v>
       </c>
@@ -23459,7 +23463,7 @@
       </c>
       <c r="BE138" s="2"/>
     </row>
-    <row r="139" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>45857</v>
       </c>
@@ -23614,7 +23618,7 @@
       </c>
       <c r="BE139" s="2"/>
     </row>
-    <row r="140" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>45857</v>
       </c>
@@ -23769,7 +23773,7 @@
       </c>
       <c r="BE140" s="2"/>
     </row>
-    <row r="141" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="6">
         <v>45857</v>
       </c>
@@ -23921,7 +23925,7 @@
       </c>
       <c r="BE141" s="8"/>
     </row>
-    <row r="142" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>45857</v>
       </c>
@@ -24076,7 +24080,7 @@
       </c>
       <c r="BE142" s="2"/>
     </row>
-    <row r="143" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>45857</v>
       </c>
@@ -24231,7 +24235,7 @@
       </c>
       <c r="BE143" s="2"/>
     </row>
-    <row r="144" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>45857</v>
       </c>
@@ -24386,7 +24390,7 @@
       </c>
       <c r="BE144" s="2"/>
     </row>
-    <row r="145" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>45857</v>
       </c>
@@ -24541,7 +24545,7 @@
       </c>
       <c r="BE145" s="2"/>
     </row>
-    <row r="146" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>45857</v>
       </c>
@@ -24696,7 +24700,7 @@
       </c>
       <c r="BE146" s="2"/>
     </row>
-    <row r="147" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="6">
         <v>45857</v>
       </c>
@@ -24851,7 +24855,7 @@
       </c>
       <c r="BE147" s="8"/>
     </row>
-    <row r="148" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>45857</v>
       </c>
@@ -25006,7 +25010,7 @@
       </c>
       <c r="BE148" s="2"/>
     </row>
-    <row r="149" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>45857</v>
       </c>
@@ -25161,7 +25165,7 @@
       </c>
       <c r="BE149" s="2"/>
     </row>
-    <row r="150" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>45857</v>
       </c>
@@ -25316,7 +25320,7 @@
       </c>
       <c r="BE150" s="2"/>
     </row>
-    <row r="151" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>45857</v>
       </c>
@@ -25471,7 +25475,7 @@
       </c>
       <c r="BE151" s="2"/>
     </row>
-    <row r="152" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>45857</v>
       </c>
@@ -25626,7 +25630,7 @@
       </c>
       <c r="BE152" s="2"/>
     </row>
-    <row r="153" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>45857</v>
       </c>
@@ -25781,7 +25785,7 @@
       </c>
       <c r="BE153" s="2"/>
     </row>
-    <row r="154" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="6">
         <v>45857</v>
       </c>
@@ -25936,7 +25940,7 @@
       </c>
       <c r="BE154" s="8"/>
     </row>
-    <row r="155" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>45857</v>
       </c>
@@ -26091,7 +26095,7 @@
       </c>
       <c r="BE155" s="2"/>
     </row>
-    <row r="156" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>45857</v>
       </c>
@@ -26246,7 +26250,7 @@
       </c>
       <c r="BE156" s="2"/>
     </row>
-    <row r="157" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>45857</v>
       </c>
@@ -26401,7 +26405,7 @@
       </c>
       <c r="BE157" s="2"/>
     </row>
-    <row r="158" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>45857</v>
       </c>
@@ -26556,7 +26560,7 @@
       </c>
       <c r="BE158" s="2"/>
     </row>
-    <row r="159" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>45857</v>
       </c>
@@ -26711,7 +26715,7 @@
       </c>
       <c r="BE159" s="2"/>
     </row>
-    <row r="160" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>45857</v>
       </c>
@@ -26866,7 +26870,7 @@
       </c>
       <c r="BE160" s="2"/>
     </row>
-    <row r="161" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>45857</v>
       </c>
@@ -27021,7 +27025,7 @@
       </c>
       <c r="BE161" s="2"/>
     </row>
-    <row r="162" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>45857</v>
       </c>
@@ -27176,7 +27180,7 @@
       </c>
       <c r="BE162" s="2"/>
     </row>
-    <row r="163" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>45857</v>
       </c>
@@ -27331,7 +27335,7 @@
       </c>
       <c r="BE163" s="2"/>
     </row>
-    <row r="164" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="6">
         <v>45857</v>
       </c>
@@ -27486,7 +27490,7 @@
       </c>
       <c r="BE164" s="8"/>
     </row>
-    <row r="165" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>45857</v>
       </c>
@@ -27641,7 +27645,7 @@
       </c>
       <c r="BE165" s="2"/>
     </row>
-    <row r="166" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>45857</v>
       </c>
@@ -27796,7 +27800,7 @@
       </c>
       <c r="BE166" s="2"/>
     </row>
-    <row r="167" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>45857</v>
       </c>
@@ -27951,7 +27955,7 @@
       </c>
       <c r="BE167" s="2"/>
     </row>
-    <row r="168" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>45857</v>
       </c>
@@ -28106,7 +28110,7 @@
       </c>
       <c r="BE168" s="2"/>
     </row>
-    <row r="169" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>45857</v>
       </c>
@@ -28261,7 +28265,7 @@
       </c>
       <c r="BE169" s="2"/>
     </row>
-    <row r="170" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="6">
         <v>45857</v>
       </c>
@@ -28416,7 +28420,7 @@
       </c>
       <c r="BE170" s="8"/>
     </row>
-    <row r="171" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>45857</v>
       </c>
@@ -28571,7 +28575,7 @@
       </c>
       <c r="BE171" s="2"/>
     </row>
-    <row r="172" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>45857</v>
       </c>
@@ -28726,7 +28730,7 @@
       </c>
       <c r="BE172" s="2"/>
     </row>
-    <row r="173" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>45857</v>
       </c>
@@ -28881,7 +28885,7 @@
       </c>
       <c r="BE173" s="2"/>
     </row>
-    <row r="174" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>45857</v>
       </c>
@@ -29036,7 +29040,7 @@
       </c>
       <c r="BE174" s="2"/>
     </row>
-    <row r="175" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>45857</v>
       </c>
@@ -29191,7 +29195,7 @@
       </c>
       <c r="BE175" s="2"/>
     </row>
-    <row r="176" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="6">
         <v>45857</v>
       </c>
@@ -29346,7 +29350,7 @@
       </c>
       <c r="BE176" s="8"/>
     </row>
-    <row r="177" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>45857</v>
       </c>
@@ -29501,7 +29505,7 @@
       </c>
       <c r="BE177" s="2"/>
     </row>
-    <row r="178" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>45857</v>
       </c>
@@ -29656,7 +29660,7 @@
       </c>
       <c r="BE178" s="2"/>
     </row>
-    <row r="179" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>45857</v>
       </c>
@@ -29811,7 +29815,7 @@
       </c>
       <c r="BE179" s="2"/>
     </row>
-    <row r="180" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>45857</v>
       </c>
@@ -29966,7 +29970,7 @@
       </c>
       <c r="BE180" s="2"/>
     </row>
-    <row r="181" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>45857</v>
       </c>
@@ -30121,7 +30125,7 @@
       </c>
       <c r="BE181" s="2"/>
     </row>
-    <row r="182" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>45857</v>
       </c>
@@ -30276,7 +30280,7 @@
       </c>
       <c r="BE182" s="2"/>
     </row>
-    <row r="183" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>45857</v>
       </c>
@@ -30431,7 +30435,7 @@
       </c>
       <c r="BE183" s="2"/>
     </row>
-    <row r="184" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:57" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="6">
         <v>45857</v>
       </c>
@@ -30586,7 +30590,7 @@
       </c>
       <c r="BE184" s="8"/>
     </row>
-    <row r="185" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>45857</v>
       </c>
@@ -30741,7 +30745,7 @@
       </c>
       <c r="BE185" s="2"/>
     </row>
-    <row r="186" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>45857</v>
       </c>
@@ -30896,7 +30900,7 @@
       </c>
       <c r="BE186" s="2"/>
     </row>
-    <row r="187" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>45857</v>
       </c>
@@ -31051,7 +31055,7 @@
       </c>
       <c r="BE187" s="2"/>
     </row>
-    <row r="188" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>45857</v>
       </c>
@@ -31206,7 +31210,7 @@
       </c>
       <c r="BE188" s="2"/>
     </row>
-    <row r="189" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>45857</v>
       </c>
@@ -31361,7 +31365,7 @@
       </c>
       <c r="BE189" s="2"/>
     </row>
-    <row r="190" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>45857</v>
       </c>
@@ -31516,7 +31520,7 @@
       </c>
       <c r="BE190" s="2"/>
     </row>
-    <row r="191" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>45857</v>
       </c>
@@ -31671,7 +31675,7 @@
       </c>
       <c r="BE191" s="2"/>
     </row>
-    <row r="192" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>45857</v>
       </c>
@@ -31826,7 +31830,7 @@
       </c>
       <c r="BE192" s="2"/>
     </row>
-    <row r="193" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>45857</v>
       </c>

</xml_diff>